<commit_message>
wrap up session summary 1.6.21
</commit_message>
<xml_diff>
--- a/Workflow/משימות.xlsx
+++ b/Workflow/משימות.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Matlab\docs\temporal_segmentation\Workflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avner\Documents\2ndDegree\Project\temporal_segmentation\Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586F6315-A9FA-493E-BDBE-0AE5F42B1285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252EBB74-2C4E-49CE-B626-1EFFA9453C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
   <si>
     <t>משימה</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>תעדוף</t>
+  </si>
+  <si>
+    <t>סיכום סשן עבודה - 1.6.21</t>
   </si>
 </sst>
 </file>
@@ -191,7 +194,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -521,21 +524,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="41.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.8984375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -561,7 +564,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -587,7 +590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -613,7 +616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -639,7 +642,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -665,7 +668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -685,13 +688,13 @@
         <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -711,13 +714,13 @@
         <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="H7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -737,13 +740,13 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="H8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -769,7 +772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -795,7 +798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -821,7 +824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -847,7 +850,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -873,7 +876,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -899,7 +902,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
contrast measure + resources
</commit_message>
<xml_diff>
--- a/Workflow/משימות.xlsx
+++ b/Workflow/משימות.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Matlab\docs\temporal_segmentation\Workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586F6315-A9FA-493E-BDBE-0AE5F42B1285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA441E3-89BE-4215-A1A2-1B3828B6D650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,17 +522,17 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G6" sqref="A6:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" customWidth="1"/>
+    <col min="4" max="4" width="8.796875" customWidth="1"/>
     <col min="5" max="5" width="41.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.8984375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="30.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>